<commit_message>
testing more levels, added debug section with "k" command to kill all enemies on screen
</commit_message>
<xml_diff>
--- a/data/level_template.xlsx
+++ b/data/level_template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NPS\CS3021\BigProject\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkh0208/Documents/GitHub/bomberman/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FF0403-4572-0240-BFE1-958234A74DF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12330"/>
+    <workbookView xWindow="1060" yWindow="1020" windowWidth="29720" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="13">
   <si>
     <t>W</t>
   </si>
@@ -57,12 +58,18 @@
   </si>
   <si>
     <t>breakable gfx</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +116,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -122,13 +135,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,24 +423,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="18" width="3.140625" customWidth="1"/>
+    <col min="1" max="17" width="5.33203125" customWidth="1"/>
+    <col min="18" max="18" width="3.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>17</v>
       </c>
       <c r="B1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -437,7 +453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,7 +748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,132 +762,117 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="J14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="K14" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="L14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="M14" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="N14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O14" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="P14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="Q14" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="4" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="J18" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="B19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="B20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="B21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="B22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>